<commit_message>
add tipo_proyecto to general table
</commit_message>
<xml_diff>
--- a/Horas_Equipo.xlsx
+++ b/Horas_Equipo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniqueyanbal-my.sharepoint.com/personal/carlos_gamero_yanbal_com/Documents/Documentos/Yanbal/Equipo/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniqueyanbal-my.sharepoint.com/personal/carlos_gamero_yanbal_com/Documents/Documentos/Yanbal/Equipo/dashboard_control_horas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{2F83B730-268D-40BA-8F94-FB9925A76D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCC55C31-81AA-4AA0-8AA5-2D703EC38170}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{2F83B730-268D-40BA-8F94-FB9925A76D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B113E2F-928B-468A-BE5C-649BF97A61BC}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8865" windowWidth="29040" windowHeight="15840" xr2:uid="{F33FE17F-1C3A-4A55-A144-5A389564AA0B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
   <si>
     <t>Run MAM</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Adolfo Espinoza (c)</t>
+  </si>
+  <si>
+    <t>Run DataLake</t>
   </si>
 </sst>
 </file>
@@ -293,15 +296,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5ABB344-3121-4007-AF53-47F3BBE7B595}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,7 +883,7 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>40</v>
       </c>
       <c r="G8" s="1">
@@ -1419,52 +1419,52 @@
       </c>
       <c r="E21" s="1">
         <f>SUM(F21:O21)</f>
-        <v>800</v>
+        <v>640</v>
       </c>
       <c r="F21" s="1">
-        <f>40*4*50%</f>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" ref="G21:O22" si="1">40*4*50%</f>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>40*4*40%</f>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -1473,116 +1473,116 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1">
         <f>SUM(F22:O22)</f>
-        <v>800</v>
+        <v>320</v>
       </c>
       <c r="F22" s="1">
-        <f>40*4*50%</f>
-        <v>80</v>
+        <f>40*4*20%</f>
+        <v>32</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f t="shared" ref="G22:O22" si="1">40*4*20%</f>
+        <v>32</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ref="E23" si="2">SUM(F23:O23)</f>
-        <v>1280</v>
+        <f>SUM(F23:O23)</f>
+        <v>960</v>
       </c>
       <c r="F23" s="1">
-        <f>40*4*80%</f>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:O24" si="3">40*4*80%</f>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -1591,10 +1591,10 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ref="E24:E27" si="4">SUM(F24:O24)</f>
+        <f t="shared" ref="E24" si="2">SUM(F24:O24)</f>
         <v>1280</v>
       </c>
       <c r="F24" s="1">
@@ -1602,7 +1602,7 @@
         <v>128</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G24:O25" si="3">40*4*80%</f>
         <v>128</v>
       </c>
       <c r="H24" s="1">
@@ -1642,7 +1642,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -1651,58 +1651,58 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="4"/>
-        <v>960</v>
+        <f t="shared" ref="E25:E28" si="4">SUM(F25:O25)</f>
+        <v>1280</v>
       </c>
       <c r="F25" s="1">
-        <f>40*4*60%</f>
-        <v>96</v>
+        <f>40*4*80%</f>
+        <v>128</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" ref="G25:O27" si="5">40*4*60%</f>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="5"/>
-        <v>96</v>
+        <f t="shared" si="3"/>
+        <v>128</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
@@ -1711,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="4"/>
@@ -1722,7 +1722,7 @@
         <v>96</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G26:O28" si="5">40*4*60%</f>
         <v>96</v>
       </c>
       <c r="H26" s="1">
@@ -1760,7 +1760,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -1769,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="4"/>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
@@ -1827,56 +1827,56 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1">
-        <f>SUM(F28:O28)</f>
-        <v>1280</v>
+        <f t="shared" si="4"/>
+        <v>960</v>
       </c>
       <c r="F28" s="1">
-        <f>40*4*80%</f>
-        <v>128</v>
+        <f>40*4*60%</f>
+        <v>96</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" ref="G28:O29" si="6">40*4*80%</f>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="6"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
@@ -1885,7 +1885,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1">
         <f>SUM(F29:O29)</f>
@@ -1896,7 +1896,7 @@
         <v>128</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G29:O30" si="6">40*4*80%</f>
         <v>128</v>
       </c>
       <c r="H29" s="1">
@@ -1928,6 +1928,64 @@
         <v>128</v>
       </c>
       <c r="O29" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1">
+        <f>SUM(F30:O30)</f>
+        <v>1280</v>
+      </c>
+      <c r="F30" s="1">
+        <f>40*4*80%</f>
+        <v>128</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="O30" s="1">
         <f t="shared" si="6"/>
         <v>128</v>
       </c>

</xml_diff>